<commit_message>
added strategies on conv_v2
</commit_message>
<xml_diff>
--- a/vivadoHLS2019/conv/conv (v2).xlsx
+++ b/vivadoHLS2019/conv/conv (v2).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chenq\MAG\code\FFF\HLS2019\conv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95D1842-F3B4-45A7-80F0-62852ABF4F08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417BE9C5-E9C7-4122-BC23-269468E4123A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-22046" yWindow="-9" windowWidth="22149" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="76">
   <si>
     <t>conv</t>
   </si>
@@ -197,12 +197,6 @@
     <t>Filter_2_p_ap</t>
   </si>
   <si>
-    <t>WRp_ap</t>
-  </si>
-  <si>
-    <t>WCp_ap</t>
-  </si>
-  <si>
     <t>S</t>
   </si>
   <si>
@@ -255,6 +249,21 @@
   </si>
   <si>
     <t xml:space="preserve"> viri na FPGA</t>
+  </si>
+  <si>
+    <t>W_Row_pipeline_ap_v2</t>
+  </si>
+  <si>
+    <t>W_Col_pipeline_ap_v2</t>
+  </si>
+  <si>
+    <t>W_Row_pipeline_ap_d3_c</t>
+  </si>
+  <si>
+    <t>W_Col_pipeline_ap_d3_c</t>
+  </si>
+  <si>
+    <t>Filter_2_p_ap_v2</t>
   </si>
 </sst>
 </file>
@@ -595,10 +604,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection activeCell="A46" sqref="A46"/>
-      <selection pane="topRight" activeCell="H125" sqref="H125"/>
+      <selection pane="topRight" activeCell="I149" sqref="I149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,9 +618,11 @@
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" customWidth="1"/>
-    <col min="8" max="10" width="18.28515625" customWidth="1"/>
-    <col min="11" max="11" width="19.5703125" customWidth="1"/>
+    <col min="7" max="7" width="26" customWidth="1"/>
+    <col min="8" max="8" width="24.85546875" customWidth="1"/>
+    <col min="9" max="9" width="26" customWidth="1"/>
+    <col min="10" max="10" width="24.140625" customWidth="1"/>
+    <col min="11" max="11" width="23.140625" customWidth="1"/>
     <col min="12" max="12" width="18.42578125" customWidth="1"/>
     <col min="13" max="13" width="16.85546875" customWidth="1"/>
     <col min="14" max="14" width="15.85546875" customWidth="1"/>
@@ -635,7 +646,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -890,7 +901,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B20">
         <f>SUM(B15:B18)</f>
@@ -927,7 +938,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22">
@@ -957,7 +968,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23">
@@ -987,7 +998,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24">
@@ -1017,7 +1028,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25">
@@ -1047,7 +1058,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26">
@@ -1092,7 +1103,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28">
@@ -1126,7 +1137,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B29" s="1"/>
       <c r="E29">
@@ -1156,29 +1167,29 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B31" s="1"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B32" s="1"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E36">
         <f>E26/C26</f>
@@ -1203,7 +1214,7 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E37">
         <f>(C12/E12)</f>
@@ -1253,7 +1264,7 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E40">
         <f>E37/E29</f>
@@ -1542,7 +1553,7 @@
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B57" s="1"/>
       <c r="E57" s="1">
@@ -1768,7 +1779,7 @@
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B64">
         <f>SUM(B59:B62)</f>
@@ -1825,7 +1836,7 @@
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C67">
         <f>C59/B59*100</f>
@@ -1878,7 +1889,7 @@
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C68">
         <f>C60/B60*100</f>
@@ -1931,7 +1942,7 @@
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C69">
         <f>C61/B61*100</f>
@@ -1984,7 +1995,7 @@
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C70">
         <f>C62/B62*100</f>
@@ -2037,7 +2048,7 @@
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C71">
         <f>SUM(C67:C70)/4</f>
@@ -2094,7 +2105,7 @@
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E72">
         <f>E71/C71</f>
@@ -2464,7 +2475,7 @@
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B101">
         <f>SUM(B96:B99)</f>
@@ -2515,7 +2526,7 @@
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C103">
         <f>C96/B96*100</f>
@@ -2548,7 +2559,7 @@
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B104" s="1"/>
       <c r="C104">
@@ -2582,7 +2593,7 @@
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B105" s="1"/>
       <c r="C105">
@@ -2616,7 +2627,7 @@
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C106">
         <f t="shared" si="7"/>
@@ -2649,7 +2660,7 @@
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C107">
         <f>SUM(C103:C106)/4</f>
@@ -2694,7 +2705,7 @@
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F108">
         <f>F107/C107</f>
@@ -2723,7 +2734,7 @@
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F111">
         <f>(C92/F92)</f>
@@ -2779,10 +2790,10 @@
         <v>4.2846078793618387</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J116" s="1"/>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>0</v>
       </c>
@@ -2795,7 +2806,7 @@
       <c r="H117" s="1"/>
       <c r="I117" s="1"/>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C118" s="1" t="s">
         <v>1</v>
       </c>
@@ -2803,13 +2814,22 @@
         <v>52</v>
       </c>
       <c r="G118" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="H118" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="I118" t="s">
+        <v>75</v>
+      </c>
+      <c r="J118" t="s">
+        <v>71</v>
+      </c>
+      <c r="K118" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>6</v>
       </c>
@@ -2817,13 +2837,13 @@
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B120" s="1"/>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>30</v>
       </c>
@@ -2831,8 +2851,11 @@
       <c r="F121" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I121" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>11</v>
       </c>
@@ -2840,8 +2863,11 @@
       <c r="G122" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J122" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>12</v>
       </c>
@@ -2849,14 +2875,17 @@
       <c r="H123" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K123" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B124" s="1"/>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>14</v>
       </c>
@@ -2870,20 +2899,29 @@
       <c r="H125" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I125" t="s">
+        <v>51</v>
+      </c>
+      <c r="J125" t="s">
+        <v>51</v>
+      </c>
+      <c r="K125" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B126" s="1"/>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B127" s="1"/>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>17</v>
       </c>
@@ -2900,17 +2938,26 @@
       <c r="H128">
         <v>437537</v>
       </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I128">
+        <v>9745</v>
+      </c>
+      <c r="J128">
+        <v>172305</v>
+      </c>
+      <c r="K128">
+        <v>197473</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B130" s="1"/>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C131" s="1"/>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>18</v>
       </c>
@@ -2929,8 +2976,17 @@
       <c r="H132">
         <v>6</v>
       </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I132">
+        <v>0</v>
+      </c>
+      <c r="J132">
+        <v>20</v>
+      </c>
+      <c r="K132">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>19</v>
       </c>
@@ -2949,8 +3005,17 @@
       <c r="H133">
         <v>7</v>
       </c>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I133">
+        <v>58</v>
+      </c>
+      <c r="J133">
+        <v>25</v>
+      </c>
+      <c r="K133">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>20</v>
       </c>
@@ -2969,8 +3034,17 @@
       <c r="H134">
         <v>1144</v>
       </c>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I134">
+        <v>14582</v>
+      </c>
+      <c r="J134">
+        <v>3337</v>
+      </c>
+      <c r="K134">
+        <v>1421</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>21</v>
       </c>
@@ -2989,10 +3063,19 @@
       <c r="H135">
         <v>1699</v>
       </c>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I135">
+        <v>13085</v>
+      </c>
+      <c r="J135">
+        <v>4661</v>
+      </c>
+      <c r="K135">
+        <v>1822</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B137">
         <f>SUM(B132:B135)</f>
@@ -3014,8 +3097,20 @@
         <f>SUM(H132:H135)</f>
         <v>2856</v>
       </c>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I137">
+        <f t="shared" ref="I137:K137" si="22">SUM(I132:I135)</f>
+        <v>27725</v>
+      </c>
+      <c r="J137">
+        <f t="shared" si="22"/>
+        <v>8043</v>
+      </c>
+      <c r="K137">
+        <f t="shared" si="22"/>
+        <v>3256</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -3025,9 +3120,9 @@
       <c r="G138" s="1"/>
       <c r="H138" s="1"/>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B140" s="1"/>
       <c r="C140" s="1">
@@ -3048,86 +3143,130 @@
         <f>H132/B132*100</f>
         <v>2.1428571428571428</v>
       </c>
-      <c r="I140" s="1"/>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I140" s="1">
+        <f>I132/B132*100</f>
+        <v>0</v>
+      </c>
+      <c r="J140">
+        <f>J132/B132*100</f>
+        <v>7.1428571428571423</v>
+      </c>
+      <c r="K140">
+        <f>K132/B132*100</f>
+        <v>2.1428571428571428</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B141" s="1"/>
       <c r="C141" s="1">
-        <f t="shared" ref="C141:C143" si="22">C133/B133*100</f>
+        <f t="shared" ref="C141:C143" si="23">C133/B133*100</f>
         <v>2.2727272727272729</v>
       </c>
       <c r="D141" s="1"/>
       <c r="E141" s="1"/>
       <c r="F141" s="1">
-        <f t="shared" ref="F141:F143" si="23">F133/B133*100</f>
+        <f t="shared" ref="F141:F143" si="24">F133/B133*100</f>
         <v>25.454545454545453</v>
       </c>
       <c r="G141" s="1">
-        <f t="shared" ref="G141:G143" si="24">G133/B133*100</f>
+        <f t="shared" ref="G141:G143" si="25">G133/B133*100</f>
         <v>2.7272727272727271</v>
       </c>
       <c r="H141" s="1">
-        <f t="shared" ref="H141:H143" si="25">H133/B133*100</f>
+        <f>H133/B133*100</f>
         <v>3.1818181818181817</v>
       </c>
-      <c r="I141" s="1"/>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I141" s="1">
+        <f t="shared" ref="I141:I143" si="26">I133/B133*100</f>
+        <v>26.36363636363636</v>
+      </c>
+      <c r="J141">
+        <f t="shared" ref="J141:J144" si="27">J133/B133*100</f>
+        <v>11.363636363636363</v>
+      </c>
+      <c r="K141">
+        <f t="shared" ref="K141:K143" si="28">K133/B133*100</f>
+        <v>3.1818181818181817</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B142" s="1"/>
       <c r="C142" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.69830827067669177</v>
       </c>
       <c r="D142" s="1"/>
       <c r="E142" s="1"/>
       <c r="F142" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>13.671052631578947</v>
       </c>
       <c r="G142" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>2.2208646616541357</v>
       </c>
       <c r="H142" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" ref="H141:H143" si="29">H134/B134*100</f>
         <v>1.0751879699248119</v>
       </c>
-      <c r="I142" s="1"/>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I142" s="1">
+        <f t="shared" si="26"/>
+        <v>13.704887218045112</v>
+      </c>
+      <c r="J142">
+        <f t="shared" si="27"/>
+        <v>3.1362781954887216</v>
+      </c>
+      <c r="K142">
+        <f t="shared" si="28"/>
+        <v>1.3355263157894737</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B143" s="1"/>
       <c r="C143" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>2.9511278195488719</v>
       </c>
       <c r="D143" s="1"/>
       <c r="E143" s="1"/>
       <c r="F143" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>24.900375939849624</v>
       </c>
       <c r="G143" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>4.3082706766917296</v>
       </c>
       <c r="H143" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>3.1936090225563909</v>
       </c>
-      <c r="I143" s="1"/>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I143" s="1">
+        <f t="shared" si="26"/>
+        <v>24.595864661654137</v>
+      </c>
+      <c r="J143">
+        <f t="shared" si="27"/>
+        <v>8.7612781954887211</v>
+      </c>
+      <c r="K143">
+        <f t="shared" si="28"/>
+        <v>3.4248120300751883</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B144" s="1"/>
       <c r="C144" s="1">
@@ -3137,22 +3276,33 @@
       <c r="D144" s="1"/>
       <c r="E144" s="1"/>
       <c r="F144" s="1">
-        <f t="shared" ref="F144:H144" si="26">SUM(F140:F143)/4</f>
+        <f t="shared" ref="F144:K144" si="30">SUM(F140:F143)/4</f>
         <v>16.006493506493506</v>
       </c>
       <c r="G144" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>3.9212448735475052</v>
       </c>
       <c r="H144" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>2.3983680792891318</v>
       </c>
-      <c r="I144" s="1"/>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I144" s="1">
+        <f t="shared" si="30"/>
+        <v>16.166097060833902</v>
+      </c>
+      <c r="J144" s="1">
+        <f t="shared" si="30"/>
+        <v>7.601012474367737</v>
+      </c>
+      <c r="K144" s="1">
+        <f t="shared" si="30"/>
+        <v>2.5212534176349966</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -3170,9 +3320,20 @@
         <f>H144/C144</f>
         <v>1.4455731077723275</v>
       </c>
-      <c r="I145" s="1"/>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I145" s="1">
+        <f>I144/C144</f>
+        <v>9.7438234650393323</v>
+      </c>
+      <c r="J145">
+        <f>J144/C144</f>
+        <v>4.5813731927439392</v>
+      </c>
+      <c r="K145">
+        <f>K144/C144</f>
+        <v>1.5196400293538297</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -3183,7 +3344,7 @@
       <c r="H146" s="1"/>
       <c r="I146" s="1"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>38</v>
       </c>
@@ -3199,8 +3360,20 @@
         <f>(C128/H128)</f>
         <v>1.8103360401520328</v>
       </c>
-    </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I148">
+        <f>(C128/I128)</f>
+        <v>81.281580297588505</v>
+      </c>
+      <c r="J148">
+        <f>(C128/J128)</f>
+        <v>4.5970169176750533</v>
+      </c>
+      <c r="K148">
+        <f>(C128/K128)</f>
+        <v>4.0111255715971295</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>39</v>
       </c>
@@ -3209,12 +3382,24 @@
         <v>8.2931278323158981</v>
       </c>
       <c r="G149">
-        <f t="shared" ref="G149:H149" si="27">G148/G145</f>
+        <f t="shared" ref="G149:K149" si="31">G148/G145</f>
         <v>0.80141285377288307</v>
       </c>
       <c r="H149">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>1.2523310169637951</v>
+      </c>
+      <c r="I149">
+        <f t="shared" si="31"/>
+        <v>8.3418568274790061</v>
+      </c>
+      <c r="J149">
+        <f t="shared" si="31"/>
+        <v>1.0034146366761587</v>
+      </c>
+      <c r="K149">
+        <f t="shared" si="31"/>
+        <v>2.6395235016958005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>